<commit_message>
- x designators for used defintions
</commit_message>
<xml_diff>
--- a/qualityOfLife-definitions.xlsx
+++ b/qualityOfLife-definitions.xlsx
@@ -59,7 +59,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t> Definition</t>
+    <t>Definition</t>
   </si>
   <si>
     <t>Definition Source</t>
@@ -108,7 +108,7 @@
     <t>2 questions to assess ability to dress and groom one's self. 2 questions: one question on help of devices and one on help of a person.</t>
   </si>
   <si>
-    <t>dressing &amp; grooming x - dress</t>
+    <t>dressing &amp; grooming - dress</t>
   </si>
   <si>
     <t>to dress</t>
@@ -120,7 +120,7 @@
     <t>&lt;</t>
   </si>
   <si>
-    <t>dressing &amp; grooming x - shampoo</t>
+    <t>dressing &amp; grooming - shampoo</t>
   </si>
   <si>
     <t>to shampoo</t>
@@ -129,7 +129,7 @@
     <t>CL448079</t>
   </si>
   <si>
-    <t>dressing &amp; grooming x - aids</t>
+    <t>dressing &amp; grooming - aids</t>
   </si>
   <si>
     <t>aids of a person or device</t>
@@ -144,7 +144,7 @@
     <t>2 questions to assess ability to get up out of bed or a chair. 2 questions: one question on help of devices and one on help of a person.</t>
   </si>
   <si>
-    <t>arising x - chair</t>
+    <t>arising - chair</t>
   </si>
   <si>
     <t>from chair</t>
@@ -153,7 +153,7 @@
     <t>C1290946</t>
   </si>
   <si>
-    <t>arising x - bed</t>
+    <t>arising - bed</t>
   </si>
   <si>
     <t>from bed</t>
@@ -162,7 +162,7 @@
     <t>C0439549</t>
   </si>
   <si>
-    <t>arising x - aids</t>
+    <t>arising - aids</t>
   </si>
   <si>
     <t>eating</t>
@@ -171,7 +171,7 @@
     <t>3 questions to assess ability to use utencils, lift a glass or open a milk carton. 2 questions: one question on help of devices and one on help of a person.</t>
   </si>
   <si>
-    <t>eating x - cut</t>
+    <t>eating - cut</t>
   </si>
   <si>
     <t>cut meat</t>
@@ -180,7 +180,7 @@
     <t>CL448082</t>
   </si>
   <si>
-    <t>eating x - open</t>
+    <t>eating - open</t>
   </si>
   <si>
     <t>milk carton</t>
@@ -189,7 +189,7 @@
     <t>CL448084</t>
   </si>
   <si>
-    <t>eating x - lift</t>
+    <t>eating - lift</t>
   </si>
   <si>
     <t>glass to mouth</t>
@@ -198,7 +198,7 @@
     <t>CL448083</t>
   </si>
   <si>
-    <t>eating x - aids</t>
+    <t>eating - aids</t>
   </si>
   <si>
     <t>walking</t>
@@ -207,7 +207,7 @@
     <t>2 questions to assess ability walking on flat grounds and climbs up stairs. 2 questions: one question on help of devices and one on help of a person.</t>
   </si>
   <si>
-    <t>walking x - climb steps</t>
+    <t>walking - climb steps</t>
   </si>
   <si>
     <t>climb steps</t>
@@ -216,7 +216,7 @@
     <t>CL448086</t>
   </si>
   <si>
-    <t>walking x - walk</t>
+    <t>walking - walk</t>
   </si>
   <si>
     <t>walk outdoors on flat ground</t>
@@ -225,7 +225,7 @@
     <t>CL448085</t>
   </si>
   <si>
-    <t>walking x - aids</t>
+    <t>walking - aids</t>
   </si>
   <si>
     <t>hygiene</t>
@@ -234,7 +234,7 @@
     <t>3 questions to assess ability to wash body, get off toilet and take a bath. 2 questions: one question on help of devices and one on help of a person.</t>
   </si>
   <si>
-    <t>hygiene x - bath</t>
+    <t>hygiene - bath</t>
   </si>
   <si>
     <t>take bath</t>
@@ -243,7 +243,7 @@
     <t>CL448101</t>
   </si>
   <si>
-    <t>hygiene x - wash</t>
+    <t>hygiene - wash</t>
   </si>
   <si>
     <t>wash and dry body</t>
@@ -252,7 +252,7 @@
     <t>CL448100</t>
   </si>
   <si>
-    <t>hygiene x - toilet</t>
+    <t>hygiene - toilet</t>
   </si>
   <si>
     <t>get off the toilet</t>
@@ -261,7 +261,7 @@
     <t>CL448102</t>
   </si>
   <si>
-    <t>hygiene x - aids</t>
+    <t>hygiene - aids</t>
   </si>
   <si>
     <t>reach</t>
@@ -270,7 +270,7 @@
     <t>2 questions to assess ability to lift 5 lb objects overhead or on the ground. 2 questions: one question on help of devices and one on help of a person.</t>
   </si>
   <si>
-    <t>reach x - pick up</t>
+    <t>reach - pick up</t>
   </si>
   <si>
     <t>pick up from floor</t>
@@ -279,7 +279,7 @@
     <t>CL448104</t>
   </si>
   <si>
-    <t>reach x - from above</t>
+    <t>reach - from above</t>
   </si>
   <si>
     <t>object from above head</t>
@@ -288,7 +288,7 @@
     <t>CL448103</t>
   </si>
   <si>
-    <t>reach x - aids</t>
+    <t>reach - aids</t>
   </si>
   <si>
     <t>grip</t>
@@ -297,7 +297,7 @@
     <t>3 questions to assess ability to open car doors or previously opened jars. 2 questions: one question on help of devices and one on help of a person.</t>
   </si>
   <si>
-    <t>grip x - faucets</t>
+    <t>grip - faucets</t>
   </si>
   <si>
     <t>faucets</t>
@@ -306,7 +306,7 @@
     <t>CL448107</t>
   </si>
   <si>
-    <t>grip x - car doors</t>
+    <t>grip - car doors</t>
   </si>
   <si>
     <t>open car doors</t>
@@ -315,7 +315,7 @@
     <t>CL448105</t>
   </si>
   <si>
-    <t>grip x - jars</t>
+    <t>grip - jars</t>
   </si>
   <si>
     <t>open jars</t>
@@ -324,7 +324,7 @@
     <t>CL448106</t>
   </si>
   <si>
-    <t>grip x - aids</t>
+    <t>grip - aids</t>
   </si>
   <si>
     <t>common daily activities</t>
@@ -333,7 +333,7 @@
     <t>3 questions to assess ability to perform common errands, getting in and out of cars, or doing light chores. 2 questions: one question on help of devices and one on help of a person.</t>
   </si>
   <si>
-    <t>common daily activities x - vacuum</t>
+    <t>common daily activities - vacuum</t>
   </si>
   <si>
     <t>vacuum</t>
@@ -342,7 +342,7 @@
     <t>CL448110</t>
   </si>
   <si>
-    <t>common daily activities x - errands</t>
+    <t>common daily activities - errands</t>
   </si>
   <si>
     <t>errands</t>
@@ -351,7 +351,7 @@
     <t>CL448108</t>
   </si>
   <si>
-    <t>common daily activities x - out of car</t>
+    <t>common daily activities - out of car</t>
   </si>
   <si>
     <t>get out of the car</t>
@@ -360,7 +360,7 @@
     <t>CL448109</t>
   </si>
   <si>
-    <t>common daily activities x - aids</t>
+    <t>common daily activities - aids</t>
   </si>
 </sst>
 </file>
@@ -752,10 +752,10 @@
   </sheetPr>
   <dimension ref="A1:IY38"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>